<commit_message>
atualizacion 2 semana,nuevo  tiempo de estudio 80%
</commit_message>
<xml_diff>
--- a/cronograma mes.xlsx
+++ b/cronograma mes.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5053EE5-A3FC-481F-A52E-F86C4C56BB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF60503C-2512-482C-B56E-D42CD15B6FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Programación semanal de tareas" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="First_Day">Hoja1!#REF!</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="80">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -224,6 +225,54 @@
   </si>
   <si>
     <t xml:space="preserve">domingo/lunes </t>
+  </si>
+  <si>
+    <t>2da semana</t>
+  </si>
+  <si>
+    <t>hacer ejercicios de calculo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">horas que no se pueden modificar </t>
+  </si>
+  <si>
+    <t>20h</t>
+  </si>
+  <si>
+    <t>horas de taller</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>horas de estudio</t>
+  </si>
+  <si>
+    <t>17h</t>
+  </si>
+  <si>
+    <t>hora de estudio al 80%</t>
+  </si>
+  <si>
+    <t>14h</t>
+  </si>
+  <si>
+    <t>posibles horas a eliminar</t>
+  </si>
+  <si>
+    <t>4h</t>
+  </si>
+  <si>
+    <t>vi ejercicios de algebra</t>
+  </si>
+  <si>
+    <t>los termine en la noche anterior</t>
+  </si>
+  <si>
+    <t>aproveche para comprar cosas pendientes de un proyecto</t>
+  </si>
+  <si>
+    <t>ejercicios mecanica</t>
   </si>
 </sst>
 </file>
@@ -431,7 +480,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="45">
+  <fills count="48">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -680,6 +729,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor theme="9" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1007,7 +1074,7 @@
     <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1184,6 +1251,63 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="39" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="39" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="39" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="37" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="37" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="37" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1193,59 +1317,27 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="45" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="39" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="39" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="39" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="37" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="37" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="37" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="47">
@@ -1297,7 +1389,7 @@
     <cellStyle name="Título 3" xfId="9" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="22" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="76">
     <dxf>
       <font>
         <b val="0"/>
@@ -2374,6 +2466,13 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -2400,13 +2499,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -2448,6 +2540,1156 @@
         </horizontal>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="&quot;Completada&quot;;&quot; &quot;;&quot; &quot;"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="&quot;Completada&quot;;&quot; &quot;;&quot; &quot;"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="&quot;Completada&quot;;&quot; &quot;;&quot; &quot;"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="&quot;Completada&quot;;&quot; &quot;;&quot; &quot;"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="&quot;Completada&quot;;&quot; &quot;;&quot; &quot;"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="&quot;Completada&quot;;&quot; &quot;;&quot; &quot;"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="&quot;Completada&quot;;&quot; &quot;;&quot; &quot;"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="&quot;Completada&quot;;&quot; &quot;;&quot; &quot;"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="&quot;Completada&quot;;&quot; &quot;;&quot; &quot;"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="0"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0"/>
+        </horizontal>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2462,25 +3704,50 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_Schedule" displayName="Table_Schedule" ref="B12:R38" headerRowCount="0" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_Schedule" displayName="Table_Schedule" ref="B12:R38" headerRowCount="0" totalsRowShown="0" headerRowDxfId="75" dataDxfId="73" headerRowBorderDxfId="74" tableBorderDxfId="72">
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Tarea" headerRowDxfId="33" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Quién" headerRowDxfId="31" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Completada" headerRowDxfId="29" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quién2" headerRowDxfId="27" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Completada " headerRowDxfId="25" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Quién3" headerRowDxfId="23" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Completada  " headerRowDxfId="21" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Quién4" headerRowDxfId="19" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Completada   " headerRowDxfId="17" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Quién5" headerRowDxfId="15" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Completada    " headerRowDxfId="13" dataDxfId="12"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Quién6" headerRowDxfId="11" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Completada     " headerRowDxfId="9" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Quién7" headerRowDxfId="7" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Completada      " headerRowDxfId="5" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{F3061868-0AFF-4CA0-BB23-4E0E7C31B881}" name="Columna1" headerRowDxfId="3" dataDxfId="2"/>
-    <tableColumn id="17" xr3:uid="{3DEA49A8-B94B-47FF-8C09-879AA1C3801C}" name="Columna2" headerRowDxfId="1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Tarea" headerRowDxfId="71" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Quién" headerRowDxfId="69" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Completada" headerRowDxfId="67" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quién2" headerRowDxfId="65" dataDxfId="64"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Completada " headerRowDxfId="63" dataDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Quién3" headerRowDxfId="61" dataDxfId="60"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Completada  " headerRowDxfId="59" dataDxfId="58"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Quién4" headerRowDxfId="57" dataDxfId="56"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Completada   " headerRowDxfId="55" dataDxfId="54"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Quién5" headerRowDxfId="53" dataDxfId="52"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Completada    " headerRowDxfId="51" dataDxfId="50"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Quién6" headerRowDxfId="49" dataDxfId="48"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Completada     " headerRowDxfId="47" dataDxfId="46"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Quién7" headerRowDxfId="45" dataDxfId="44"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Completada      " headerRowDxfId="43" dataDxfId="42"/>
+    <tableColumn id="16" xr3:uid="{F3061868-0AFF-4CA0-BB23-4E0E7C31B881}" name="Columna1" headerRowDxfId="41" dataDxfId="40"/>
+    <tableColumn id="17" xr3:uid="{3DEA49A8-B94B-47FF-8C09-879AA1C3801C}" name="Columna2" headerRowDxfId="39" dataDxfId="38"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D8D0ACE6-453B-4628-9C3B-96FA1597D058}" name="Table_Schedule3" displayName="Table_Schedule3" ref="B7:R33" headerRowCount="0" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36" headerRowBorderDxfId="34" tableBorderDxfId="35">
+  <tableColumns count="17">
+    <tableColumn id="1" xr3:uid="{FAD4D9DC-9D36-4275-ACAC-4CC4348BEF36}" name="Tarea" headerRowDxfId="33" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{5478FB7D-5690-4E4F-8958-F158CC827E42}" name="Quién" headerRowDxfId="31" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{9A179E77-3317-441F-B265-5707E33F0FB5}" name="Completada" headerRowDxfId="29" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{C9D17EF0-B477-4350-BF43-AA3D05B9FC89}" name="Quién2" headerRowDxfId="27" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{498CD2AB-8DD8-4E80-9D2A-9DBCA5EB36D6}" name="Completada " headerRowDxfId="25" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{ACDBB9A6-DC9C-4722-B09A-95A7D8D956CC}" name="Quién3" headerRowDxfId="23" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{864DE25B-BD72-41F9-B2CA-843BA4E229EC}" name="Completada  " headerRowDxfId="21" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{C9A91230-668B-4633-AE46-956283A16980}" name="Quién4" headerRowDxfId="19" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{8124C4CF-5EB9-419D-B3B5-BAC77774ABF2}" name="Completada   " headerRowDxfId="17" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{2C77B670-2A48-4F25-93C6-0B2E90C5C56E}" name="Quién5" headerRowDxfId="15" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{894E42CB-A1D9-477D-A456-90A177248053}" name="Completada    " headerRowDxfId="13" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{89CBFB81-F3FB-4EAA-B752-4CB7790E9785}" name="Quién6" headerRowDxfId="11" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{7B40B1AF-582A-406D-B6F3-A245E5233025}" name="Completada     " headerRowDxfId="9" dataDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{22B2674A-9424-4895-ABFC-B9CC086D6EA5}" name="Quién7" headerRowDxfId="7" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{02A5D974-E9CF-4168-8594-6A99A6CE31E6}" name="Completada      " headerRowDxfId="5" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{B40C91CB-880C-40AA-8DD9-6B1E35859BD2}" name="Columna1" headerRowDxfId="3" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{EE4E8AF3-28FD-4C62-BCFD-8A3380F1D038}" name="Columna2" headerRowDxfId="1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2742,8 +4009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{146E92A0-90E0-4E04-9A19-C4BAC4B5715F}">
   <dimension ref="B8:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R55" sqref="B8:R55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2778,40 +4045,40 @@
       <c r="B9" s="3"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="73"/>
-      <c r="J9" s="73"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="92"/>
+      <c r="H9" s="92"/>
+      <c r="I9" s="92"/>
+      <c r="J9" s="92"/>
       <c r="K9" s="12"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
-      <c r="C10" s="79" t="s">
+      <c r="C10" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="81"/>
-      <c r="G10" s="82" t="s">
+      <c r="D10" s="84"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="83"/>
-      <c r="I10" s="83"/>
-      <c r="J10" s="84"/>
-      <c r="K10" s="85" t="s">
+      <c r="H10" s="87"/>
+      <c r="I10" s="87"/>
+      <c r="J10" s="88"/>
+      <c r="K10" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="L10" s="86"/>
-      <c r="M10" s="86"/>
-      <c r="N10" s="87"/>
-      <c r="O10" s="74" t="s">
+      <c r="L10" s="90"/>
+      <c r="M10" s="90"/>
+      <c r="N10" s="91"/>
+      <c r="O10" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="P10" s="75"/>
-      <c r="Q10" s="75"/>
-      <c r="R10" s="76"/>
+      <c r="P10" s="94"/>
+      <c r="Q10" s="94"/>
+      <c r="R10" s="95"/>
     </row>
     <row r="11" spans="2:18" ht="18" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
@@ -3844,26 +5111,26 @@
       <c r="B41" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C41" s="77" t="s">
+      <c r="C41" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="D41" s="77"/>
-      <c r="E41" s="77" t="s">
+      <c r="D41" s="82"/>
+      <c r="E41" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="F41" s="77"/>
-      <c r="G41" s="77" t="s">
+      <c r="F41" s="82"/>
+      <c r="G41" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="H41" s="77"/>
-      <c r="I41" s="77" t="s">
+      <c r="H41" s="82"/>
+      <c r="I41" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="J41" s="77"/>
-      <c r="K41" s="77" t="s">
+      <c r="J41" s="82"/>
+      <c r="K41" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="L41" s="77"/>
+      <c r="L41" s="82"/>
     </row>
     <row r="42" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="15" t="s">
@@ -3884,22 +5151,22 @@
       <c r="B43" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C43" s="90" t="s">
+      <c r="C43" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="D43" s="90"/>
-      <c r="E43" s="89" t="s">
+      <c r="D43" s="81"/>
+      <c r="E43" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="F43" s="89"/>
-      <c r="G43" s="90" t="s">
+      <c r="F43" s="80"/>
+      <c r="G43" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="H43" s="90"/>
-      <c r="I43" s="89" t="s">
+      <c r="H43" s="81"/>
+      <c r="I43" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="J43" s="89"/>
+      <c r="J43" s="80"/>
       <c r="K43" s="78"/>
       <c r="L43" s="78"/>
     </row>
@@ -3907,16 +5174,16 @@
       <c r="B44" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C44" s="90"/>
-      <c r="D44" s="90"/>
+      <c r="C44" s="81"/>
+      <c r="D44" s="81"/>
       <c r="E44" s="78"/>
       <c r="F44" s="78"/>
-      <c r="G44" s="90"/>
-      <c r="H44" s="90"/>
-      <c r="I44" s="88" t="s">
+      <c r="G44" s="81"/>
+      <c r="H44" s="81"/>
+      <c r="I44" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="J44" s="88"/>
+      <c r="J44" s="77"/>
       <c r="K44" s="78"/>
       <c r="L44" s="78"/>
     </row>
@@ -3924,60 +5191,60 @@
       <c r="B45" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C45" s="88" t="s">
+      <c r="C45" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="D45" s="88"/>
-      <c r="E45" s="88" t="s">
+      <c r="D45" s="77"/>
+      <c r="E45" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="F45" s="88"/>
-      <c r="G45" s="88" t="s">
+      <c r="F45" s="77"/>
+      <c r="G45" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="H45" s="88"/>
-      <c r="I45" s="91" t="s">
+      <c r="H45" s="77"/>
+      <c r="I45" s="76" t="s">
         <v>50</v>
       </c>
-      <c r="J45" s="91"/>
-      <c r="K45" s="88" t="s">
+      <c r="J45" s="76"/>
+      <c r="K45" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="L45" s="88"/>
+      <c r="L45" s="77"/>
     </row>
     <row r="46" spans="2:18" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C46" s="88"/>
-      <c r="D46" s="88"/>
-      <c r="E46" s="88"/>
-      <c r="F46" s="88"/>
-      <c r="G46" s="88"/>
-      <c r="H46" s="88"/>
-      <c r="I46" s="91"/>
-      <c r="J46" s="91"/>
-      <c r="K46" s="88"/>
-      <c r="L46" s="88"/>
+      <c r="C46" s="77"/>
+      <c r="D46" s="77"/>
+      <c r="E46" s="77"/>
+      <c r="F46" s="77"/>
+      <c r="G46" s="77"/>
+      <c r="H46" s="77"/>
+      <c r="I46" s="76"/>
+      <c r="J46" s="76"/>
+      <c r="K46" s="77"/>
+      <c r="L46" s="77"/>
     </row>
     <row r="47" spans="2:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C47" s="88" t="s">
+      <c r="C47" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="D47" s="88"/>
-      <c r="E47" s="88" t="s">
+      <c r="D47" s="77"/>
+      <c r="E47" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="F47" s="88"/>
-      <c r="G47" s="88" t="s">
+      <c r="F47" s="77"/>
+      <c r="G47" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="H47" s="88"/>
-      <c r="I47" s="91"/>
-      <c r="J47" s="91"/>
+      <c r="H47" s="77"/>
+      <c r="I47" s="76"/>
+      <c r="J47" s="76"/>
       <c r="K47" s="78"/>
       <c r="L47" s="78"/>
     </row>
@@ -3985,16 +5252,16 @@
       <c r="B48" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C48" s="88"/>
-      <c r="D48" s="88"/>
-      <c r="E48" s="88"/>
-      <c r="F48" s="88"/>
-      <c r="G48" s="88"/>
-      <c r="H48" s="88"/>
-      <c r="I48" s="88" t="s">
+      <c r="C48" s="77"/>
+      <c r="D48" s="77"/>
+      <c r="E48" s="77"/>
+      <c r="F48" s="77"/>
+      <c r="G48" s="77"/>
+      <c r="H48" s="77"/>
+      <c r="I48" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="J48" s="88"/>
+      <c r="J48" s="77"/>
       <c r="K48" s="78"/>
       <c r="L48" s="78"/>
     </row>
@@ -4002,22 +5269,22 @@
       <c r="B49" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C49" s="91" t="s">
+      <c r="C49" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="D49" s="91"/>
-      <c r="E49" s="91" t="s">
+      <c r="D49" s="76"/>
+      <c r="E49" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="F49" s="91"/>
-      <c r="G49" s="91" t="s">
+      <c r="F49" s="76"/>
+      <c r="G49" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="H49" s="91"/>
-      <c r="I49" s="91" t="s">
+      <c r="H49" s="76"/>
+      <c r="I49" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="J49" s="91"/>
+      <c r="J49" s="76"/>
       <c r="K49" s="78"/>
       <c r="L49" s="78"/>
     </row>
@@ -4025,14 +5292,14 @@
       <c r="B50" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C50" s="91"/>
-      <c r="D50" s="91"/>
-      <c r="E50" s="91"/>
-      <c r="F50" s="91"/>
-      <c r="G50" s="91"/>
-      <c r="H50" s="91"/>
-      <c r="I50" s="91"/>
-      <c r="J50" s="91"/>
+      <c r="C50" s="76"/>
+      <c r="D50" s="76"/>
+      <c r="E50" s="76"/>
+      <c r="F50" s="76"/>
+      <c r="G50" s="76"/>
+      <c r="H50" s="76"/>
+      <c r="I50" s="76"/>
+      <c r="J50" s="76"/>
       <c r="K50" s="78"/>
       <c r="L50" s="78"/>
     </row>
@@ -4040,20 +5307,20 @@
       <c r="B51" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C51" s="91" t="s">
+      <c r="C51" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="D51" s="91"/>
-      <c r="E51" s="89" t="s">
+      <c r="D51" s="76"/>
+      <c r="E51" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="F51" s="89"/>
-      <c r="G51" s="91" t="s">
+      <c r="F51" s="80"/>
+      <c r="G51" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="H51" s="91"/>
-      <c r="I51" s="92"/>
-      <c r="J51" s="92"/>
+      <c r="H51" s="76"/>
+      <c r="I51" s="79"/>
+      <c r="J51" s="79"/>
       <c r="K51" s="78"/>
       <c r="L51" s="78"/>
     </row>
@@ -4061,16 +5328,16 @@
       <c r="B52" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C52" s="91"/>
-      <c r="D52" s="91"/>
-      <c r="E52" s="91" t="s">
+      <c r="C52" s="76"/>
+      <c r="D52" s="76"/>
+      <c r="E52" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="F52" s="91"/>
-      <c r="G52" s="91"/>
-      <c r="H52" s="91"/>
-      <c r="I52" s="92"/>
-      <c r="J52" s="92"/>
+      <c r="F52" s="76"/>
+      <c r="G52" s="76"/>
+      <c r="H52" s="76"/>
+      <c r="I52" s="79"/>
+      <c r="J52" s="79"/>
       <c r="K52" s="78"/>
       <c r="L52" s="78"/>
     </row>
@@ -4080,12 +5347,12 @@
       </c>
       <c r="C53" s="78"/>
       <c r="D53" s="78"/>
-      <c r="E53" s="91"/>
-      <c r="F53" s="91"/>
+      <c r="E53" s="76"/>
+      <c r="F53" s="76"/>
       <c r="G53" s="78"/>
       <c r="H53" s="78"/>
-      <c r="I53" s="92"/>
-      <c r="J53" s="92"/>
+      <c r="I53" s="79"/>
+      <c r="J53" s="79"/>
       <c r="K53" s="78"/>
       <c r="L53" s="78"/>
     </row>
@@ -4099,10 +5366,10 @@
       <c r="F54" s="78"/>
       <c r="G54" s="78"/>
       <c r="H54" s="78"/>
-      <c r="I54" s="88" t="s">
+      <c r="I54" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="J54" s="88"/>
+      <c r="J54" s="77"/>
       <c r="K54" s="78"/>
       <c r="L54" s="78"/>
     </row>
@@ -4110,19 +5377,64 @@
       <c r="B55" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C55" s="93"/>
-      <c r="D55" s="94"/>
-      <c r="E55" s="93"/>
-      <c r="F55" s="94"/>
-      <c r="G55" s="93"/>
-      <c r="H55" s="94"/>
-      <c r="I55" s="88"/>
-      <c r="J55" s="88"/>
-      <c r="K55" s="93"/>
-      <c r="L55" s="94"/>
+      <c r="C55" s="74"/>
+      <c r="D55" s="75"/>
+      <c r="E55" s="74"/>
+      <c r="F55" s="75"/>
+      <c r="G55" s="74"/>
+      <c r="H55" s="75"/>
+      <c r="I55" s="77"/>
+      <c r="J55" s="77"/>
+      <c r="K55" s="74"/>
+      <c r="L55" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="61">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="O10:R10"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="K45:L46"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="K49:L49"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="I45:J47"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="E52:F53"/>
+    <mergeCell ref="C43:D44"/>
+    <mergeCell ref="C49:D50"/>
+    <mergeCell ref="C45:D46"/>
+    <mergeCell ref="C47:D48"/>
+    <mergeCell ref="E49:F50"/>
+    <mergeCell ref="E47:F48"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F46"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="G43:H44"/>
+    <mergeCell ref="G45:H46"/>
+    <mergeCell ref="G47:H48"/>
+    <mergeCell ref="G49:H50"/>
+    <mergeCell ref="G51:H52"/>
     <mergeCell ref="C55:D55"/>
     <mergeCell ref="E55:F55"/>
     <mergeCell ref="G55:H55"/>
@@ -4139,51 +5451,6 @@
     <mergeCell ref="C53:D53"/>
     <mergeCell ref="C51:D52"/>
     <mergeCell ref="I51:J53"/>
-    <mergeCell ref="E45:F46"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="G43:H44"/>
-    <mergeCell ref="G45:H46"/>
-    <mergeCell ref="G47:H48"/>
-    <mergeCell ref="G49:H50"/>
-    <mergeCell ref="G51:H52"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="E52:F53"/>
-    <mergeCell ref="C43:D44"/>
-    <mergeCell ref="C49:D50"/>
-    <mergeCell ref="C45:D46"/>
-    <mergeCell ref="C47:D48"/>
-    <mergeCell ref="E49:F50"/>
-    <mergeCell ref="E47:F48"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="I45:J47"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="K41:L41"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="K45:L46"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="K47:L47"/>
-    <mergeCell ref="K48:L48"/>
-    <mergeCell ref="K49:L49"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="O10:R10"/>
-    <mergeCell ref="C41:D41"/>
   </mergeCells>
   <phoneticPr fontId="24" type="noConversion"/>
   <dataValidations count="1">
@@ -4240,7 +5507,1611 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B5A0037-0B6B-48E9-96B4-3A146FAE4567}">
+  <dimension ref="A3:R50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="40.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B3" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="7"/>
+    </row>
+    <row r="4" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B4" s="3"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="92"/>
+      <c r="I4" s="92"/>
+      <c r="J4" s="92"/>
+      <c r="K4" s="12"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B5" s="3"/>
+      <c r="C5" s="83" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="86" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="89" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="90"/>
+      <c r="M5" s="90"/>
+      <c r="N5" s="91"/>
+      <c r="O5" s="93" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" s="94"/>
+      <c r="Q5" s="94"/>
+      <c r="R5" s="95"/>
+    </row>
+    <row r="6" spans="2:18" ht="18" x14ac:dyDescent="0.3">
+      <c r="B6" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="P6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="R6" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B7" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="22">
+        <v>2</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="17"/>
+      <c r="G7" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="22">
+        <v>2</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" s="17"/>
+      <c r="K7" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" s="22">
+        <v>2</v>
+      </c>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="P7" s="22">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B8" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="22">
+        <v>2</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="22">
+        <v>2</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="J8" s="17"/>
+      <c r="K8" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" s="22">
+        <v>2</v>
+      </c>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="P8" s="22">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="26"/>
+      <c r="R8" s="26"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B9" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="22">
+        <v>2</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="22">
+        <v>2</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="K9" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" s="22">
+        <v>2</v>
+      </c>
+      <c r="M9" s="23"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="P9" s="22">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="26"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B10" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="22">
+        <v>2</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="22">
+        <v>2</v>
+      </c>
+      <c r="I10" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" s="27"/>
+      <c r="K10" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" s="22">
+        <v>2</v>
+      </c>
+      <c r="M10" s="23"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="P10" s="22">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="26"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B11" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="54">
+        <v>2</v>
+      </c>
+      <c r="E11" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="56"/>
+      <c r="G11" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="54">
+        <v>2</v>
+      </c>
+      <c r="I11" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11" s="58"/>
+      <c r="K11" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="L11" s="54">
+        <v>2</v>
+      </c>
+      <c r="M11" s="55"/>
+      <c r="N11" s="59"/>
+      <c r="O11" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="P11" s="54">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="60"/>
+      <c r="R11" s="61"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B12" s="67"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="70"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="72"/>
+      <c r="O12" s="70"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="49"/>
+      <c r="R12" s="50"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B13" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="62">
+        <v>2</v>
+      </c>
+      <c r="E13" s="63" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="64"/>
+      <c r="G13" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="62">
+        <v>2</v>
+      </c>
+      <c r="I13" s="63" t="s">
+        <v>55</v>
+      </c>
+      <c r="J13" s="105"/>
+      <c r="K13" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="62">
+        <v>2</v>
+      </c>
+      <c r="M13" s="64"/>
+      <c r="N13" s="64"/>
+      <c r="O13" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="P13" s="62">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="66"/>
+      <c r="R13" s="66"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B14" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="22">
+        <v>2</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="22">
+        <v>2</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14" s="17"/>
+      <c r="K14" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="L14" s="22">
+        <v>2</v>
+      </c>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="P14" s="22">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="26"/>
+      <c r="R14" s="26"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B15" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="22">
+        <v>2</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="22">
+        <v>2</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="J15" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="K15" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="L15" s="22">
+        <v>2</v>
+      </c>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="P15" s="22">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="26"/>
+      <c r="R15" s="26"/>
+    </row>
+    <row r="16" spans="2:18" ht="33" x14ac:dyDescent="0.3">
+      <c r="B16" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="22">
+        <v>1</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="22">
+        <v>1</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="J16" s="104" t="s">
+        <v>78</v>
+      </c>
+      <c r="K16" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="L16" s="22">
+        <v>1</v>
+      </c>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="P16" s="22">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="26"/>
+      <c r="R16" s="26"/>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B17" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="22">
+        <v>2</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="22">
+        <v>2</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="J17" s="17"/>
+      <c r="K17" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="L17" s="22">
+        <v>2</v>
+      </c>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="P17" s="22">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="26"/>
+      <c r="R17" s="26"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B18" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="22">
+        <v>1</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="22">
+        <v>1</v>
+      </c>
+      <c r="I18" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="J18" s="17"/>
+      <c r="K18" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="L18" s="22">
+        <v>1</v>
+      </c>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="P18" s="22">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="26"/>
+      <c r="R18" s="26"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B19" s="31"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="44"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="43"/>
+      <c r="P19" s="33"/>
+      <c r="Q19" s="45"/>
+      <c r="R19" s="41"/>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B20" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="22">
+        <v>2</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="22">
+        <v>2</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="J20" s="17"/>
+      <c r="K20" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="L20" s="22">
+        <v>2</v>
+      </c>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="P20" s="22">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="26"/>
+      <c r="R20" s="26"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B21" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="22">
+        <v>2</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="17"/>
+      <c r="G21" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" s="22">
+        <v>2</v>
+      </c>
+      <c r="I21" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="J21" s="17"/>
+      <c r="K21" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="L21" s="22">
+        <v>2</v>
+      </c>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="P21" s="22">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="26"/>
+      <c r="R21" s="26"/>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B22" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="22">
+        <v>2</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G22" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" s="22">
+        <v>2</v>
+      </c>
+      <c r="I22" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="J22" s="17"/>
+      <c r="K22" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="L22" s="22">
+        <v>2</v>
+      </c>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="P22" s="22">
+        <v>2</v>
+      </c>
+      <c r="Q22" s="26"/>
+      <c r="R22" s="26"/>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B23" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="22">
+        <v>2</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="17"/>
+      <c r="G23" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" s="22">
+        <v>2</v>
+      </c>
+      <c r="I23" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="J23" s="17"/>
+      <c r="K23" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="L23" s="22">
+        <v>2</v>
+      </c>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="P23" s="22">
+        <v>2</v>
+      </c>
+      <c r="Q23" s="26"/>
+      <c r="R23" s="26"/>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B24" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="22">
+        <v>2</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" s="17"/>
+      <c r="G24" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="22">
+        <v>2</v>
+      </c>
+      <c r="I24" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="J24" s="27"/>
+      <c r="K24" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="L24" s="22">
+        <v>2</v>
+      </c>
+      <c r="M24" s="23"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="P24" s="22">
+        <v>2</v>
+      </c>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="26"/>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B25" s="31"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="34"/>
+      <c r="N25" s="39"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="33"/>
+      <c r="Q25" s="40"/>
+      <c r="R25" s="41"/>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B26" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="22">
+        <v>2</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="G26" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="22">
+        <v>2</v>
+      </c>
+      <c r="I26" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="J26" s="64" t="s">
+        <v>77</v>
+      </c>
+      <c r="K26" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="L26" s="22">
+        <v>2</v>
+      </c>
+      <c r="M26" s="23"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="P26" s="22">
+        <v>2</v>
+      </c>
+      <c r="Q26" s="25"/>
+      <c r="R26" s="26"/>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B27" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="22">
+        <v>2</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" s="17"/>
+      <c r="G27" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="22">
+        <v>2</v>
+      </c>
+      <c r="I27" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="J27" s="27"/>
+      <c r="K27" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="L27" s="22">
+        <v>2</v>
+      </c>
+      <c r="M27" s="23"/>
+      <c r="N27" s="28"/>
+      <c r="O27" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="P27" s="22">
+        <v>2</v>
+      </c>
+      <c r="Q27" s="25"/>
+      <c r="R27" s="26"/>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B28" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="22">
+        <v>2</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G28" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="22">
+        <v>2</v>
+      </c>
+      <c r="I28" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="J28" s="27"/>
+      <c r="K28" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="L28" s="22">
+        <v>2</v>
+      </c>
+      <c r="M28" s="23"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="P28" s="22">
+        <v>2</v>
+      </c>
+      <c r="Q28" s="25"/>
+      <c r="R28" s="26"/>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B29" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="22">
+        <v>1</v>
+      </c>
+      <c r="E29" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" s="17"/>
+      <c r="G29" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" s="22">
+        <v>1</v>
+      </c>
+      <c r="I29" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="J29" s="27"/>
+      <c r="K29" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="L29" s="22">
+        <v>1</v>
+      </c>
+      <c r="M29" s="23"/>
+      <c r="N29" s="28"/>
+      <c r="O29" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="P29" s="22">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="25"/>
+      <c r="R29" s="26"/>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B30" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="22">
+        <v>3</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F30" s="17"/>
+      <c r="G30" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30" s="22">
+        <v>3</v>
+      </c>
+      <c r="I30" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="J30" s="27"/>
+      <c r="K30" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="L30" s="22">
+        <v>3</v>
+      </c>
+      <c r="M30" s="23"/>
+      <c r="N30" s="28"/>
+      <c r="O30" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="P30" s="22">
+        <v>3</v>
+      </c>
+      <c r="Q30" s="25"/>
+      <c r="R30" s="26"/>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B31" s="31"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="36"/>
+      <c r="L31" s="33"/>
+      <c r="M31" s="34"/>
+      <c r="N31" s="39"/>
+      <c r="O31" s="36"/>
+      <c r="P31" s="33"/>
+      <c r="Q31" s="40"/>
+      <c r="R31" s="41"/>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B32" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="22">
+        <v>2</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" s="17"/>
+      <c r="G32" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="22">
+        <v>2</v>
+      </c>
+      <c r="I32" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="J32" s="27"/>
+      <c r="K32" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="L32" s="22">
+        <v>2</v>
+      </c>
+      <c r="M32" s="23"/>
+      <c r="N32" s="28"/>
+      <c r="O32" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="P32" s="22">
+        <v>2</v>
+      </c>
+      <c r="Q32" s="26"/>
+      <c r="R32" s="26"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B33" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="29"/>
+      <c r="D33" s="22">
+        <v>4</v>
+      </c>
+      <c r="E33" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="30"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="30"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="28"/>
+      <c r="O33" s="30"/>
+      <c r="P33" s="22"/>
+      <c r="Q33" s="26"/>
+      <c r="R33" s="26"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="82" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="82"/>
+      <c r="E36" s="82" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="82"/>
+      <c r="G36" s="82" t="s">
+        <v>19</v>
+      </c>
+      <c r="H36" s="82"/>
+      <c r="I36" s="82" t="s">
+        <v>20</v>
+      </c>
+      <c r="J36" s="82"/>
+      <c r="K36" s="82" t="s">
+        <v>17</v>
+      </c>
+      <c r="L36" s="82"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B37" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="78"/>
+      <c r="D37" s="78"/>
+      <c r="E37" s="78"/>
+      <c r="F37" s="78"/>
+      <c r="G37" s="78"/>
+      <c r="H37" s="78"/>
+      <c r="I37" s="78"/>
+      <c r="J37" s="78"/>
+      <c r="K37" s="78"/>
+      <c r="L37" s="78"/>
+      <c r="M37" s="98" t="s">
+        <v>66</v>
+      </c>
+      <c r="N37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B38" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="96" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="96"/>
+      <c r="E38" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="F38" s="80"/>
+      <c r="G38" s="96" t="s">
+        <v>1</v>
+      </c>
+      <c r="H38" s="96"/>
+      <c r="I38" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="J38" s="80"/>
+      <c r="K38" s="78"/>
+      <c r="L38" s="78"/>
+      <c r="M38" s="100" t="s">
+        <v>68</v>
+      </c>
+      <c r="N38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B39" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="96"/>
+      <c r="D39" s="96"/>
+      <c r="E39" s="78"/>
+      <c r="F39" s="78"/>
+      <c r="G39" s="96"/>
+      <c r="H39" s="96"/>
+      <c r="I39" s="102" t="s">
+        <v>48</v>
+      </c>
+      <c r="J39" s="102"/>
+      <c r="K39" s="78"/>
+      <c r="L39" s="78"/>
+      <c r="M39" s="101" t="s">
+        <v>70</v>
+      </c>
+      <c r="N39" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B40" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" s="77" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="77"/>
+      <c r="E40" s="77" t="s">
+        <v>53</v>
+      </c>
+      <c r="F40" s="77"/>
+      <c r="G40" s="77" t="s">
+        <v>5</v>
+      </c>
+      <c r="H40" s="77"/>
+      <c r="I40" s="97" t="s">
+        <v>50</v>
+      </c>
+      <c r="J40" s="97"/>
+      <c r="K40" s="99" t="s">
+        <v>52</v>
+      </c>
+      <c r="L40" s="99"/>
+      <c r="M40" t="s">
+        <v>72</v>
+      </c>
+      <c r="N40" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B41" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" s="77"/>
+      <c r="D41" s="77"/>
+      <c r="E41" s="77"/>
+      <c r="F41" s="77"/>
+      <c r="G41" s="77"/>
+      <c r="H41" s="77"/>
+      <c r="I41" s="97"/>
+      <c r="J41" s="97"/>
+      <c r="K41" s="99"/>
+      <c r="L41" s="99"/>
+      <c r="M41" s="103" t="s">
+        <v>74</v>
+      </c>
+      <c r="N41" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B42" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" s="77" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" s="77"/>
+      <c r="E42" s="77" t="s">
+        <v>48</v>
+      </c>
+      <c r="F42" s="77"/>
+      <c r="G42" s="77" t="s">
+        <v>7</v>
+      </c>
+      <c r="H42" s="77"/>
+      <c r="I42" s="97"/>
+      <c r="J42" s="97"/>
+      <c r="K42" s="78"/>
+      <c r="L42" s="78"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B43" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" s="77"/>
+      <c r="D43" s="77"/>
+      <c r="E43" s="77"/>
+      <c r="F43" s="77"/>
+      <c r="G43" s="77"/>
+      <c r="H43" s="77"/>
+      <c r="I43" s="102" t="s">
+        <v>48</v>
+      </c>
+      <c r="J43" s="102"/>
+      <c r="K43" s="78"/>
+      <c r="L43" s="78"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B44" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" s="97" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44" s="97"/>
+      <c r="E44" s="97" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44" s="97"/>
+      <c r="G44" s="97" t="s">
+        <v>44</v>
+      </c>
+      <c r="H44" s="97"/>
+      <c r="I44" s="97" t="s">
+        <v>8</v>
+      </c>
+      <c r="J44" s="97"/>
+      <c r="K44" s="78"/>
+      <c r="L44" s="78"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B45" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C45" s="97"/>
+      <c r="D45" s="97"/>
+      <c r="E45" s="97"/>
+      <c r="F45" s="97"/>
+      <c r="G45" s="97"/>
+      <c r="H45" s="97"/>
+      <c r="I45" s="97"/>
+      <c r="J45" s="97"/>
+      <c r="K45" s="78"/>
+      <c r="L45" s="78"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B46" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" s="97" t="s">
+        <v>45</v>
+      </c>
+      <c r="D46" s="97"/>
+      <c r="E46" s="80" t="s">
+        <v>49</v>
+      </c>
+      <c r="F46" s="80"/>
+      <c r="G46" s="97" t="s">
+        <v>45</v>
+      </c>
+      <c r="H46" s="97"/>
+      <c r="I46" s="79"/>
+      <c r="J46" s="79"/>
+      <c r="K46" s="78"/>
+      <c r="L46" s="78"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B47" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47" s="97"/>
+      <c r="D47" s="97"/>
+      <c r="E47" s="97" t="s">
+        <v>46</v>
+      </c>
+      <c r="F47" s="97"/>
+      <c r="G47" s="97"/>
+      <c r="H47" s="97"/>
+      <c r="I47" s="79"/>
+      <c r="J47" s="79"/>
+      <c r="K47" s="78"/>
+      <c r="L47" s="78"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B48" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C48" s="78"/>
+      <c r="D48" s="78"/>
+      <c r="E48" s="97"/>
+      <c r="F48" s="97"/>
+      <c r="G48" s="78"/>
+      <c r="H48" s="78"/>
+      <c r="I48" s="79"/>
+      <c r="J48" s="79"/>
+      <c r="K48" s="78"/>
+      <c r="L48" s="78"/>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B49" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49" s="78"/>
+      <c r="D49" s="78"/>
+      <c r="E49" s="78"/>
+      <c r="F49" s="78"/>
+      <c r="G49" s="78"/>
+      <c r="H49" s="78"/>
+      <c r="I49" s="102" t="s">
+        <v>53</v>
+      </c>
+      <c r="J49" s="102"/>
+      <c r="K49" s="78"/>
+      <c r="L49" s="78"/>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B50" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50" s="74"/>
+      <c r="D50" s="75"/>
+      <c r="E50" s="74"/>
+      <c r="F50" s="75"/>
+      <c r="G50" s="74"/>
+      <c r="H50" s="75"/>
+      <c r="I50" s="102"/>
+      <c r="J50" s="102"/>
+      <c r="K50" s="74"/>
+      <c r="L50" s="75"/>
+    </row>
+  </sheetData>
+  <mergeCells count="61">
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="I49:J50"/>
+    <mergeCell ref="K49:L49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="C46:D47"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:H47"/>
+    <mergeCell ref="I46:J48"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="E47:F48"/>
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="G42:H43"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="C44:D45"/>
+    <mergeCell ref="E44:F45"/>
+    <mergeCell ref="G44:H45"/>
+    <mergeCell ref="I44:J45"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="C40:D41"/>
+    <mergeCell ref="E40:F41"/>
+    <mergeCell ref="G40:H41"/>
+    <mergeCell ref="I40:J42"/>
+    <mergeCell ref="K40:L41"/>
+    <mergeCell ref="C42:D43"/>
+    <mergeCell ref="E42:F43"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="C38:D39"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="G38:H39"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="O5:R5"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="K5:N5"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba cada tarea en esta columna." sqref="B6" xr:uid="{73BF6C76-4A77-4281-97E8-ED58B176AEF7}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="2" id="{58CE87CC-33CD-4A01-8E66-85685E8C8522}">
+            <x14:iconSet iconSet="3Symbols2" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>I13:I23 I7:I11 E13:E23 E7:E11 Q7:R7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{955AE3EF-3AB6-4E52-BF0B-729B0F09A14A}">
+            <x14:iconSet iconSet="3Symbols2" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>I26:I33 E26:E33</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DEEA25CC0A0AC24199CDC46C25B8B0BC" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3b47856d4cf355c0dacb39e1084d14f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="6dc4bcd6-49db-4c07-9060-8acfc67cef9f" xmlns:ns3="fb0879af-3eba-417a-a55a-ffe6dcd6ca77" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a845a615265fdb1f7b12cc65ac20ecbd" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4448,25 +7319,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61D8B24C-3B85-4379-80DC-A0BB54E539A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E60A8B6F-A245-4A02-AD66-F6A27855DC90}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA919527-0680-40C7-8319-A14A2B99BD22}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4484,22 +7355,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E60A8B6F-A245-4A02-AD66-F6A27855DC90}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61D8B24C-3B85-4379-80DC-A0BB54E539A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>